<commit_message>
adjustments based on review
</commit_message>
<xml_diff>
--- a/biblioteka_probna.xlsx
+++ b/biblioteka_probna.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sliwimag\PycharmProjects\branch_baza_danych_robocza\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sliwimag\PycharmProjects\DL-31-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13896" windowHeight="9036" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13896" windowHeight="9036" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="Managers" sheetId="2" r:id="rId2"/>
     <sheet name="Magazines" sheetId="3" r:id="rId3"/>
+    <sheet name="Deleted" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -1063,7 +1064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -2056,7 +2057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -2358,4 +2359,18 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adjustments of the xls reader
</commit_message>
<xml_diff>
--- a/biblioteka_probna.xlsx
+++ b/biblioteka_probna.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13896" windowHeight="9036" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13896" windowHeight="9036" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -745,9 +745,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2057,13 +2058,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="2"/>
     <col min="4" max="4" width="6.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2071,7 +2073,7 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>202</v>
       </c>
       <c r="D1" t="s">
@@ -2085,7 +2087,7 @@
       <c r="B2" t="s">
         <v>204</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>2011</v>
       </c>
       <c r="D2">
@@ -2099,7 +2101,7 @@
       <c r="B3" t="s">
         <v>204</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>2011</v>
       </c>
       <c r="D3">
@@ -2113,7 +2115,7 @@
       <c r="B4" t="s">
         <v>204</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>2011</v>
       </c>
       <c r="D4">
@@ -2127,7 +2129,7 @@
       <c r="B5" t="s">
         <v>204</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>2011</v>
       </c>
       <c r="D5">
@@ -2141,7 +2143,7 @@
       <c r="B6" t="s">
         <v>204</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>2011</v>
       </c>
       <c r="D6">
@@ -2155,7 +2157,7 @@
       <c r="B7" t="s">
         <v>204</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>2015</v>
       </c>
       <c r="D7">
@@ -2169,7 +2171,7 @@
       <c r="B8" t="s">
         <v>204</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>2015</v>
       </c>
       <c r="D8">
@@ -2183,7 +2185,7 @@
       <c r="B9" t="s">
         <v>204</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>2015</v>
       </c>
       <c r="D9">
@@ -2197,7 +2199,7 @@
       <c r="B10" t="s">
         <v>204</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>2015</v>
       </c>
       <c r="D10">
@@ -2211,7 +2213,7 @@
       <c r="B11" t="s">
         <v>204</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>2015</v>
       </c>
       <c r="D11">
@@ -2225,7 +2227,7 @@
       <c r="B12" t="s">
         <v>205</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>2017</v>
       </c>
       <c r="D12">
@@ -2239,7 +2241,7 @@
       <c r="B13" t="s">
         <v>205</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>2017</v>
       </c>
       <c r="D13">
@@ -2253,7 +2255,7 @@
       <c r="B14" t="s">
         <v>205</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>2017</v>
       </c>
       <c r="D14">
@@ -2267,7 +2269,7 @@
       <c r="B15" t="s">
         <v>205</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>2017</v>
       </c>
       <c r="D15">
@@ -2281,7 +2283,7 @@
       <c r="B16" t="s">
         <v>205</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>2013</v>
       </c>
       <c r="D16">
@@ -2295,7 +2297,7 @@
       <c r="B17" t="s">
         <v>205</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <v>2013</v>
       </c>
       <c r="D17">
@@ -2309,7 +2311,7 @@
       <c r="B18" t="s">
         <v>205</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>2013</v>
       </c>
       <c r="D18">
@@ -2323,7 +2325,7 @@
       <c r="B19" t="s">
         <v>205</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>2013</v>
       </c>
       <c r="D19">
@@ -2337,7 +2339,7 @@
       <c r="B20" t="s">
         <v>205</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>2013</v>
       </c>
       <c r="D20">
@@ -2358,6 +2360,7 @@
     <hyperlink ref="B11" r:id="rId10" tooltip="Forbes" display="https://en.wikipedia.org/wiki/Forbes"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId11"/>
 </worksheet>
 </file>
 
@@ -2365,7 +2368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>

</xml_diff>